<commit_message>
ocup. hosp. & nacional & setting SE43
</commit_message>
<xml_diff>
--- a/tablas/tabla_defunciones_cero.xlsx
+++ b/tablas/tabla_defunciones_cero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\covid_cusco\tablas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F69772B-2A41-475E-9B79-2D7BFA824794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62994FC-7A5C-4A2E-A8FB-299C9579DB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B35F084E-A87D-4054-80F3-C51BCACE92B8}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Acomayo</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>26sep-9oct</t>
+  </si>
+  <si>
+    <t>SE-43</t>
+  </si>
+  <si>
+    <t>24oct-30oct</t>
   </si>
 </sst>
 </file>
@@ -523,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{994E6999-8BCD-4B3C-B1C7-C4CF1750CA02}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="J17" sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +541,7 @@
     <col min="2" max="6" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -545,8 +551,9 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>17</v>
@@ -572,8 +579,11 @@
       <c r="I2" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
         <v>16</v>
@@ -599,8 +609,11 @@
       <c r="I3" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,8 +627,9 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,8 +647,9 @@
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -648,8 +663,9 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -669,8 +685,9 @@
       <c r="I7" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -688,8 +705,9 @@
       <c r="I8" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,8 +727,11 @@
         <v>1</v>
       </c>
       <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -738,8 +759,11 @@
       <c r="I10" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -753,8 +777,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -776,8 +801,9 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -791,8 +817,11 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -806,8 +835,9 @@
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -823,8 +853,9 @@
         <v>1</v>
       </c>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
@@ -842,6 +873,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>